<commit_message>
Updated feature locations, removed lockfile
</commit_message>
<xml_diff>
--- a/tabular/reference_feature_locations.xlsx
+++ b/tabular/reference_feature_locations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="38">
   <si>
     <t>genus</t>
   </si>
@@ -203,8 +203,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="233">
+  <cellStyleXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -446,7 +448,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="233">
+  <cellStyles count="235">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -563,6 +565,7 @@
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -679,6 +682,7 @@
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1008,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="F43" sqref="A1:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1464,31 +1468,31 @@
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>17</v>
+      <c r="C26" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D26" s="3">
-        <v>23</v>
+        <v>1421</v>
       </c>
       <c r="E26" s="3">
-        <v>2275</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D27" s="3">
-        <v>1421</v>
+        <v>199</v>
       </c>
       <c r="E27" s="3">
-        <v>2242</v>
+        <v>750</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1499,13 +1503,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D28" s="3">
-        <v>199</v>
+        <v>620</v>
       </c>
       <c r="E28" s="3">
-        <v>750</v>
+        <v>3124</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1515,14 +1519,14 @@
       <c r="B29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>12</v>
+      <c r="C29" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D29" s="3">
-        <v>620</v>
+        <v>1704</v>
       </c>
       <c r="E29" s="3">
-        <v>3124</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1532,14 +1536,14 @@
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>37</v>
+      <c r="C30" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="D30" s="3">
-        <v>1704</v>
+        <v>620</v>
       </c>
       <c r="E30" s="3">
-        <v>2351</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1549,14 +1553,14 @@
       <c r="B31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>16</v>
+      <c r="C31" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D31" s="3">
-        <v>620</v>
+        <v>1119</v>
       </c>
       <c r="E31" s="3">
-        <v>1096</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1566,14 +1570,14 @@
       <c r="B32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>17</v>
+      <c r="C32" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D32" s="3">
-        <v>1736</v>
+        <v>1038</v>
       </c>
       <c r="E32" s="3">
-        <v>3124</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1583,14 +1587,14 @@
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>32</v>
+      <c r="C33" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D33" s="3">
-        <v>1119</v>
+        <v>1</v>
       </c>
       <c r="E33" s="3">
-        <v>1703</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1600,22 +1604,22 @@
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>33</v>
+      <c r="C34" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D34" s="3">
-        <v>1038</v>
+        <v>3207</v>
       </c>
       <c r="E34" s="3">
-        <v>1118</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>18</v>
@@ -1624,24 +1628,24 @@
         <v>1</v>
       </c>
       <c r="E35" s="3">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D36" s="3">
-        <v>3207</v>
+        <v>2659</v>
       </c>
       <c r="E36" s="3">
-        <v>3214</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1652,13 +1656,13 @@
         <v>7</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D37" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E37" s="3">
-        <v>19</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1669,13 +1673,13 @@
         <v>7</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D38" s="3">
-        <v>2659</v>
+        <v>303</v>
       </c>
       <c r="E38" s="3">
-        <v>2677</v>
+        <v>554</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1686,13 +1690,13 @@
         <v>7</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D39" s="3">
-        <v>100</v>
+        <v>615</v>
       </c>
       <c r="E39" s="3">
-        <v>294</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1703,13 +1707,13 @@
         <v>7</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D40" s="3">
-        <v>303</v>
+        <v>2444</v>
       </c>
       <c r="E40" s="3">
-        <v>554</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1720,13 +1724,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D41" s="3">
-        <v>615</v>
+        <v>919</v>
       </c>
       <c r="E41" s="3">
-        <v>1136</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1737,13 +1741,13 @@
         <v>7</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D42" s="3">
-        <v>2444</v>
+        <v>919</v>
       </c>
       <c r="E42" s="3">
-        <v>2665</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1754,57 +1758,23 @@
         <v>7</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D43" s="3">
-        <v>919</v>
+        <v>1483</v>
       </c>
       <c r="E43" s="3">
         <v>2739</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="3">
-        <v>919</v>
-      </c>
-      <c r="E44" s="3">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="3">
-        <v>1483</v>
-      </c>
-      <c r="E45" s="3">
-        <v>2739</v>
-      </c>
+    <row r="48" spans="1:5">
+      <c r="B48" s="4"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="3"/>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="3"/>
+      <c r="B50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Towards a more complete and minimal build
</commit_message>
<xml_diff>
--- a/tabular/reference_feature_locations.xlsx
+++ b/tabular/reference_feature_locations.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/DNArt/Hepadnaviridae-GLUE/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C78518E-D865-EC4A-834F-4084652DF654}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="460" windowWidth="26940" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="460" windowWidth="26940" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Unused" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -145,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1034,14 +1028,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
@@ -1050,7 +1044,7 @@
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -1067,7 +1061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -1087,7 +1081,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1107,7 +1101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -1124,7 +1118,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1141,7 +1135,7 @@
         <v>2454</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1158,7 +1152,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1175,7 +1169,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1192,7 +1186,7 @@
         <v>3111</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1209,7 +1203,7 @@
         <v>2365</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1226,7 +1220,7 @@
         <v>2365</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -1246,7 +1240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -1263,7 +1257,7 @@
         <v>2536</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -1280,7 +1274,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1297,7 +1291,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="2" customFormat="1">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -1314,7 +1308,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="2" customFormat="1">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -1331,7 +1325,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" s="2" customFormat="1">
       <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1348,7 +1342,7 @@
         <v>2821</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" s="2" customFormat="1">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1365,7 +1359,7 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" s="2" customFormat="1">
       <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
@@ -1382,7 +1376,7 @@
         <v>3144</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1399,7 +1393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -1416,7 +1410,7 @@
         <v>3453</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1433,7 +1427,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -1450,7 +1444,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -1467,7 +1461,7 @@
         <v>2758</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -1484,7 +1478,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1501,7 +1495,7 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
         <v>29</v>
       </c>
@@ -1518,7 +1512,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -1535,7 +1529,7 @@
         <v>3124</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1552,7 +1546,7 @@
         <v>2351</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -1569,7 +1563,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -1586,7 +1580,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1603,7 +1597,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
         <v>29</v>
       </c>
@@ -1620,7 +1614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
         <v>29</v>
       </c>
@@ -1637,7 +1631,7 @@
         <v>3214</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
@@ -1654,7 +1648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
         <v>30</v>
       </c>
@@ -1671,7 +1665,7 @@
         <v>2677</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" s="3" t="s">
         <v>30</v>
       </c>
@@ -1688,7 +1682,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
         <v>30</v>
       </c>
@@ -1705,7 +1699,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" s="3" t="s">
         <v>30</v>
       </c>
@@ -1722,7 +1716,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" s="3" t="s">
         <v>30</v>
       </c>
@@ -1739,7 +1733,7 @@
         <v>2665</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" s="3" t="s">
         <v>30</v>
       </c>
@@ -1756,7 +1750,7 @@
         <v>2739</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" s="3" t="s">
         <v>30</v>
       </c>
@@ -1773,7 +1767,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" s="3" t="s">
         <v>30</v>
       </c>
@@ -1790,7 +1784,7 @@
         <v>2739</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="19">
       <c r="F44" s="6"/>
     </row>
   </sheetData>
@@ -1805,16 +1799,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1831,7 +1825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1848,7 +1842,7 @@
         <v>2957</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1865,7 +1859,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1882,7 +1876,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1899,7 +1893,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1916,7 +1910,7 @@
         <v>3011</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1933,7 +1927,7 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>